<commit_message>
save and fetch chart in user-chart ms
</commit_message>
<xml_diff>
--- a/microservices/download templates/src/templatesStorage/LineWithAnnotationsTemplate.xlsx
+++ b/microservices/download templates/src/templatesStorage/LineWithAnnotationsTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DORA\Documents\GitHub\SaaS23-60\microservices\download templates\src\templatesStorage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67049750-DB3A-44E0-8BAE-D1303EA4FF6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8364C3D6-48C0-41AE-85DB-49746F87284D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{46EB44D5-4E4C-4FBF-9B9B-9B8682C03FE5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Chart's Title</t>
   </si>
@@ -139,6 +139,9 @@
   <si>
     <t>lineWithAnnotations</t>
   </si>
+  <si>
+    <t>ChartName</t>
+  </si>
 </sst>
 </file>
 
@@ -215,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -247,12 +250,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -572,7 +569,7 @@
   <dimension ref="A1:BY462"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -580,12 +577,12 @@
     <col min="1" max="46" width="14.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="4" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" s="4" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -613,11 +610,14 @@
       <c r="I2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -645,11 +645,11 @@
       <c r="I3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="K3" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="6" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" s="6" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -660,7 +660,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>20</v>
       </c>
@@ -680,7 +680,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>0</v>
       </c>
@@ -700,7 +700,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>22</v>
       </c>
@@ -708,7 +708,7 @@
         <v>45.6</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>90.6</v>
       </c>
@@ -716,14 +716,14 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="17" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="18" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="19" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -6631,7 +6631,7 @@
       <c r="BY462" s="5"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="EdqXZlTZz/TducJx54CZNfEdaEaz9PufWBZGfBaCt98jfI2shY1+zFxO2zK/UlTZwu5p1whFTj3MTgmTEOzQ4A==" saltValue="D3dCbwfFmz5GQFIqhmG2vw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="V1yPZ264IkWEOL/GgqlelMhYUWZqTntvXhgRZr1yC9SkGDJF0aHXIYi/qOpd3ibLzv27MfEy4mxxfIBi4K6NcQ==" saltValue="6JbYnXOK8fdFNb5wr/ZFcQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange algorithmName="SHA-512" hashValue="grJ6j9Pg3fR0ozyFbWId1iGPDl+m/wcgohlsBFVdFPlu3vLW2Q2diNvdtQZ4Y/z885xl+QQPzwXqYSHB89EeWw==" saltValue="Iwv+UuEJEwdeanhrSECMnw==" spinCount="100000" sqref="A1:XFD2" name="Range1"/>
   </protectedRanges>

</xml_diff>